<commit_message>
Update xlsx test files
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" createdVersion="5" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -232,7 +232,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtInteger" cacheId="9" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtInteger" cacheId="9" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" createdVersion="5" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -405,7 +405,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" createdVersion="5" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -484,7 +484,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" createdVersion="5" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -564,7 +564,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" rowHeaderCaption="Pastry name">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" createdVersion="5" indent="1" rowHeaderCaption="Pastry name">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -649,7 +649,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtCollapsedFields" cacheId="4" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtCollapsedFields" cacheId="4" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" createdVersion="5" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" allDrilled="1" showAll="0" defaultSubtotal="0">
@@ -734,7 +734,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFieldAsValueAndLabel" cacheId="5" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFieldAsValueAndLabel" cacheId="5" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" createdVersion="5" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" dataField="1" showAll="0" defaultSubtotal="0">
@@ -812,7 +812,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="6" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" colHeaderCaption="Measures">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="6" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" createdVersion="5" indent="1" colHeaderCaption="Measures">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisCol" showAll="0" defaultSubtotal="0">
@@ -889,7 +889,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFilter" cacheId="7" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFilter" cacheId="7" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" createdVersion="5" indent="1">
   <x:location ref="A5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
@@ -990,7 +990,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtSort" cacheId="8" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" rowHeaderCaption="Pastry name">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtSort" cacheId="8" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" createdVersion="5" indent="1" rowHeaderCaption="Pastry name">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" sortType="ascending" defaultSubtotal="0">

</xml_diff>

<commit_message>
Fix loading and saving of pivot tables with subtotal styles. Update test files, in most cases it removes defaultSubtotal from fields that shouldn't have subtotal (e.g. fields unused in the table or data fields)
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -167,9 +167,9 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Code" defaultSubtotal="0"/>
-    <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" defaultSubtotal="0"/>
+    <x:pivotField name="Code"/>
+    <x:pivotField name="NumberOfOrders" dataField="1"/>
+    <x:pivotField name="Quality"/>
     <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
@@ -177,7 +177,7 @@
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" defaultSubtotal="0"/>
+    <x:pivotField name="BakeDate"/>
   </x:pivotFields>
   <x:rowFields count="1">
     <x:field x="0"/>
@@ -253,8 +253,8 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="NumberOfOrders" dataField="1"/>
+    <x:pivotField name="Quality" dataField="1"/>
     <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
@@ -417,9 +417,9 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Code" defaultSubtotal="0"/>
-    <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Code"/>
+    <x:pivotField name="NumberOfOrders" dataField="1"/>
+    <x:pivotField name="Quality" dataField="1"/>
     <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
@@ -427,7 +427,7 @@
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" defaultSubtotal="0"/>
+    <x:pivotField name="BakeDate"/>
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="-2"/>
@@ -496,9 +496,9 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Code" defaultSubtotal="0"/>
-    <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Code"/>
+    <x:pivotField name="NumberOfOrders" dataField="1"/>
+    <x:pivotField name="Quality" dataField="1"/>
     <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
@@ -506,7 +506,7 @@
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" defaultSubtotal="0"/>
+    <x:pivotField name="BakeDate"/>
   </x:pivotFields>
   <x:rowFields count="1">
     <x:field x="0"/>
@@ -576,9 +576,9 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Code" defaultSubtotal="0"/>
-    <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Code"/>
+    <x:pivotField name="NumberOfOrders" dataField="1"/>
+    <x:pivotField name="Quality" dataField="1"/>
     <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
@@ -586,7 +586,7 @@
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" defaultSubtotal="0"/>
+    <x:pivotField name="BakeDate"/>
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>
@@ -661,9 +661,9 @@
         <x:item sd="0" x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Code" defaultSubtotal="0"/>
-    <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Code"/>
+    <x:pivotField name="NumberOfOrders" dataField="1"/>
+    <x:pivotField name="Quality" dataField="1"/>
     <x:pivotField name="Month" axis="axisRow" allDrilled="1" showAll="0" defaultSubtotal="0">
       <x:items count="3">
         <x:item sd="0" x="0"/>
@@ -671,7 +671,7 @@
         <x:item sd="0" x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" defaultSubtotal="0"/>
+    <x:pivotField name="BakeDate"/>
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>
@@ -746,9 +746,9 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Code" defaultSubtotal="0"/>
-    <x:pivotField name="NumberOfOrders" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" defaultSubtotal="0"/>
+    <x:pivotField name="Code"/>
+    <x:pivotField name="NumberOfOrders"/>
+    <x:pivotField name="Quality"/>
     <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
@@ -756,7 +756,7 @@
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" defaultSubtotal="0"/>
+    <x:pivotField name="BakeDate"/>
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>
@@ -824,9 +824,9 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Code" defaultSubtotal="0"/>
-    <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Code"/>
+    <x:pivotField name="NumberOfOrders" dataField="1"/>
+    <x:pivotField name="Quality" dataField="1"/>
     <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
@@ -834,7 +834,7 @@
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" defaultSubtotal="0"/>
+    <x:pivotField name="BakeDate"/>
   </x:pivotFields>
   <x:rowFields count="1">
     <x:field x="-2"/>
@@ -901,8 +901,8 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Code" defaultSubtotal="0"/>
-    <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Code"/>
+    <x:pivotField name="NumberOfOrders" dataField="1"/>
     <x:pivotField name="Quality" axis="axisPage" showAll="0" defaultSubtotal="0">
       <x:items count="16">
         <x:item x="0"/>
@@ -1002,9 +1002,9 @@
         <x:item x="4"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Code" defaultSubtotal="0"/>
-    <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Code"/>
+    <x:pivotField name="NumberOfOrders" dataField="1"/>
+    <x:pivotField name="Quality" dataField="1"/>
     <x:pivotField name="Month" axis="axisRow" showAll="0" sortType="descending" defaultSubtotal="0">
       <x:items count="3">
         <x:item x="0"/>
@@ -1012,7 +1012,7 @@
         <x:item x="2"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="BakeDate" defaultSubtotal="0"/>
+    <x:pivotField name="BakeDate"/>
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>

</xml_diff>

<commit_message>
Fix blank detection and date saving for pivot fields. Blanks weren't detected correctly, if columns had blank values below last value. Date uses correct serialization (at least Excel does), so the serializatio to the pivot field values assumes that 1900 is *not* a leap year (unlike the rest of Excel). That impacts timespan and dates before 29th feb 1900.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -1951,7 +1951,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
@@ -1960,14 +1960,15 @@
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems count="3">
+      <x:sharedItems containsBlank="1" count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
         <x:s v="Jun"/>
+        <x:m/>
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1989,12 +1990,13 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5">
+      <x:sharedItems containsSemiMixedTypes="1" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5">
         <x:n v="101"/>
         <x:n v="102"/>
         <x:n v="103"/>
         <x:n v="104"/>
         <x:n v="105"/>
+        <x:m/>
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
@@ -2004,14 +2006,15 @@
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems count="3">
+      <x:sharedItems containsBlank="1" count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
         <x:s v="Jun"/>
+        <x:m/>
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15">
+      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15">
         <x:d v="2016-04-21T00:00:00"/>
         <x:d v="2016-05-03T00:00:00"/>
         <x:d v="2016-06-24T00:00:00"/>
@@ -2027,6 +2030,7 @@
         <x:d v="2017-04-22T00:00:00"/>
         <x:d v="2017-05-03T00:00:00"/>
         <x:d v="2017-06-14T00:00:00"/>
+        <x:m/>
       </x:sharedItems>
     </x:cacheField>
   </x:cacheFields>
@@ -2049,7 +2053,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
@@ -2058,14 +2062,15 @@
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems count="3">
+      <x:sharedItems containsBlank="1" count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
         <x:s v="Jun"/>
+        <x:m/>
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -2087,7 +2092,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
@@ -2096,14 +2101,15 @@
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems count="3">
+      <x:sharedItems containsBlank="1" count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
         <x:s v="Jun"/>
+        <x:m/>
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -2125,7 +2131,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
@@ -2134,14 +2140,15 @@
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems count="3">
+      <x:sharedItems containsBlank="1" count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
         <x:s v="Jun"/>
+        <x:m/>
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -2163,7 +2170,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
@@ -2172,14 +2179,15 @@
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems count="3">
+      <x:sharedItems containsBlank="1" count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
         <x:s v="Jun"/>
+        <x:m/>
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -2201,7 +2209,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
@@ -2210,14 +2218,15 @@
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems count="3">
+      <x:sharedItems containsBlank="1" count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
         <x:s v="Jun"/>
+        <x:m/>
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -2239,7 +2248,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
@@ -2248,14 +2257,15 @@
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems count="3">
+      <x:sharedItems containsBlank="1" count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
         <x:s v="Jun"/>
+        <x:m/>
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -2277,7 +2287,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
@@ -2303,14 +2313,15 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems count="3">
+      <x:sharedItems containsBlank="1" count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
         <x:s v="Jun"/>
+        <x:m/>
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15">
+      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15">
         <x:d v="2016-04-21T00:00:00"/>
         <x:d v="2016-05-03T00:00:00"/>
         <x:d v="2016-06-24T00:00:00"/>
@@ -2326,6 +2337,7 @@
         <x:d v="2017-04-22T00:00:00"/>
         <x:d v="2017-05-03T00:00:00"/>
         <x:d v="2017-06-14T00:00:00"/>
+        <x:m/>
       </x:sharedItems>
     </x:cacheField>
   </x:cacheFields>
@@ -2348,7 +2360,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
@@ -2357,14 +2369,15 @@
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems count="3">
+      <x:sharedItems containsBlank="1" count="3">
         <x:s v="Apr"/>
         <x:s v="May"/>
         <x:s v="Jun"/>
+        <x:m/>
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>

</xml_diff>

<commit_message>
Review and rework pivot cache API, refactor and document pivot caches.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -21,16 +21,8 @@
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
   <x:pivotCaches>
-    <x:pivotCache cacheId="0" r:id="rId16"/>
-    <x:pivotCache cacheId="1" r:id="rId19"/>
-    <x:pivotCache cacheId="2" r:id="rId22"/>
-    <x:pivotCache cacheId="3" r:id="rId25"/>
-    <x:pivotCache cacheId="4" r:id="rId28"/>
-    <x:pivotCache cacheId="5" r:id="rId31"/>
-    <x:pivotCache cacheId="6" r:id="rId34"/>
-    <x:pivotCache cacheId="7" r:id="rId37"/>
-    <x:pivotCache cacheId="8" r:id="rId40"/>
-    <x:pivotCache cacheId="9" r:id="rId43"/>
+    <x:pivotCache cacheId="0" r:id="rId15"/>
+    <x:pivotCache cacheId="1" r:id="rId16"/>
   </x:pivotCaches>
 </x:workbook>
 </file>
@@ -171,10 +163,11 @@
     <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Quality" defaultSubtotal="0"/>
     <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
-      <x:items count="3">
+      <x:items count="4">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
+        <x:item x="3"/>
       </x:items>
     </x:pivotField>
     <x:pivotField name="BakeDate" defaultSubtotal="0"/>
@@ -205,7 +198,7 @@
   <x:colFields count="1">
     <x:field x="4"/>
   </x:colFields>
-  <x:colItems count="4">
+  <x:colItems count="5">
     <x:i>
       <x:x v="0"/>
     </x:i>
@@ -214,6 +207,9 @@
     </x:i>
     <x:i>
       <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
     </x:i>
     <x:i t="grand">
       <x:x/>
@@ -232,7 +228,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtInteger" cacheId="9" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtInteger" cacheId="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -245,25 +241,27 @@
       </x:items>
     </x:pivotField>
     <x:pivotField name="Code" axis="axisRow" showAll="0" defaultSubtotal="0">
-      <x:items count="5">
+      <x:items count="6">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
         <x:item x="3"/>
         <x:item x="4"/>
+        <x:item x="5"/>
       </x:items>
     </x:pivotField>
     <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
-      <x:items count="3">
+      <x:items count="4">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
+        <x:item x="3"/>
       </x:items>
     </x:pivotField>
     <x:pivotField name="BakeDate" axis="axisRow" showAll="0" defaultSubtotal="0">
-      <x:items count="15">
+      <x:items count="16">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
@@ -279,6 +277,7 @@
         <x:item x="12"/>
         <x:item x="13"/>
         <x:item x="14"/>
+        <x:item x="15"/>
       </x:items>
     </x:pivotField>
   </x:pivotFields>
@@ -287,7 +286,7 @@
     <x:field x="1"/>
     <x:field x="5"/>
   </x:rowFields>
-  <x:rowItems count="28">
+  <x:rowItems count="30">
     <x:i>
       <x:x v="0"/>
     </x:i>
@@ -321,6 +320,9 @@
     <x:i>
       <x:x v="4"/>
     </x:i>
+    <x:i>
+      <x:x v="5"/>
+    </x:i>
     <x:i t="grand">
       <x:x/>
     </x:i>
@@ -368,6 +370,9 @@
     </x:i>
     <x:i>
       <x:x v="14"/>
+    </x:i>
+    <x:i>
+      <x:x v="15"/>
     </x:i>
     <x:i t="grand">
       <x:x/>
@@ -377,7 +382,7 @@
     <x:field x="4"/>
     <x:field x="-2"/>
   </x:colFields>
-  <x:colItems count="4">
+  <x:colItems count="5">
     <x:i>
       <x:x v="0"/>
     </x:i>
@@ -386,6 +391,9 @@
     </x:i>
     <x:i>
       <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
     </x:i>
     <x:i t="grand">
       <x:x/>
@@ -405,7 +413,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="1" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="0" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -421,10 +429,11 @@
     <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
-      <x:items count="3">
+      <x:items count="4">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
+        <x:item x="3"/>
       </x:items>
     </x:pivotField>
     <x:pivotField name="BakeDate" defaultSubtotal="0"/>
@@ -456,7 +465,7 @@
   <x:colFields count="1">
     <x:field x="4"/>
   </x:colFields>
-  <x:colItems count="4">
+  <x:colItems count="5">
     <x:i>
       <x:x v="0"/>
     </x:i>
@@ -465,6 +474,9 @@
     </x:i>
     <x:i>
       <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
     </x:i>
     <x:i t="grand">
       <x:x/>
@@ -484,7 +496,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="2" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -500,10 +512,11 @@
     <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
-      <x:items count="3">
+      <x:items count="4">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
+        <x:item x="3"/>
       </x:items>
     </x:pivotField>
     <x:pivotField name="BakeDate" defaultSubtotal="0"/>
@@ -535,7 +548,7 @@
     <x:field x="4"/>
     <x:field x="-2"/>
   </x:colFields>
-  <x:colItems count="4">
+  <x:colItems count="5">
     <x:i>
       <x:x v="0"/>
     </x:i>
@@ -544,6 +557,9 @@
     </x:i>
     <x:i>
       <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
     </x:i>
     <x:i t="grand">
       <x:x/>
@@ -564,7 +580,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="3" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" rowHeaderCaption="Pastry name">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtNoColumnLabels" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" rowHeaderCaption="Pastry name">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -580,10 +596,11 @@
     <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
-      <x:items count="3">
+      <x:items count="4">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
+        <x:item x="3"/>
       </x:items>
     </x:pivotField>
     <x:pivotField name="BakeDate" defaultSubtotal="0"/>
@@ -592,7 +609,7 @@
     <x:field x="0"/>
     <x:field x="4"/>
   </x:rowFields>
-  <x:rowItems count="10">
+  <x:rowItems count="11">
     <x:i>
       <x:x v="0"/>
     </x:i>
@@ -619,6 +636,9 @@
     </x:i>
     <x:i>
       <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
     </x:i>
     <x:i t="grand">
       <x:x/>
@@ -649,7 +669,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtCollapsedFields" cacheId="4" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtCollapsedFields" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" allDrilled="1" showAll="0" defaultSubtotal="0">
@@ -665,10 +685,11 @@
     <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Month" axis="axisRow" allDrilled="1" showAll="0" defaultSubtotal="0">
-      <x:items count="3">
+      <x:items count="4">
         <x:item sd="0" x="0"/>
         <x:item sd="0" x="1"/>
         <x:item sd="0" x="2"/>
+        <x:item sd="0" x="3"/>
       </x:items>
     </x:pivotField>
     <x:pivotField name="BakeDate" defaultSubtotal="0"/>
@@ -677,7 +698,7 @@
     <x:field x="0"/>
     <x:field x="4"/>
   </x:rowFields>
-  <x:rowItems count="10">
+  <x:rowItems count="11">
     <x:i>
       <x:x v="0"/>
     </x:i>
@@ -704,6 +725,9 @@
     </x:i>
     <x:i>
       <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
     </x:i>
     <x:i t="grand">
       <x:x/>
@@ -734,7 +758,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFieldAsValueAndLabel" cacheId="5" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFieldAsValueAndLabel" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" dataField="1" showAll="0" defaultSubtotal="0">
@@ -750,10 +774,11 @@
     <x:pivotField name="NumberOfOrders" defaultSubtotal="0"/>
     <x:pivotField name="Quality" defaultSubtotal="0"/>
     <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
-      <x:items count="3">
+      <x:items count="4">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
+        <x:item x="3"/>
       </x:items>
     </x:pivotField>
     <x:pivotField name="BakeDate" defaultSubtotal="0"/>
@@ -762,7 +787,7 @@
     <x:field x="0"/>
     <x:field x="4"/>
   </x:rowFields>
-  <x:rowItems count="10">
+  <x:rowItems count="11">
     <x:i>
       <x:x v="0"/>
     </x:i>
@@ -789,6 +814,9 @@
     </x:i>
     <x:i>
       <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
     </x:i>
     <x:i t="grand">
       <x:x/>
@@ -812,7 +840,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="6" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" colHeaderCaption="Measures">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtHidesubTotals" cacheId="0" dataOnRows="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" colHeaderCaption="Measures">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisCol" showAll="0" defaultSubtotal="0">
@@ -828,10 +856,11 @@
     <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Month" axis="axisCol" showAll="0" defaultSubtotal="0">
-      <x:items count="3">
+      <x:items count="4">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
+        <x:item x="3"/>
       </x:items>
     </x:pivotField>
     <x:pivotField name="BakeDate" defaultSubtotal="0"/>
@@ -843,7 +872,7 @@
     <x:field x="4"/>
     <x:field x="0"/>
   </x:colFields>
-  <x:colItems count="10">
+  <x:colItems count="11">
     <x:i>
       <x:x v="0"/>
     </x:i>
@@ -870,6 +899,9 @@
     </x:i>
     <x:i>
       <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
     </x:i>
     <x:i t="grand">
       <x:x/>
@@ -889,7 +921,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFilter" cacheId="7" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFilter" cacheId="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
@@ -924,14 +956,15 @@
       </x:items>
     </x:pivotField>
     <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
-      <x:items count="3">
+      <x:items count="4">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
+        <x:item x="3"/>
       </x:items>
     </x:pivotField>
     <x:pivotField name="BakeDate" axis="axisPage" showAll="0" defaultSubtotal="0">
-      <x:items count="15">
+      <x:items count="16">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
@@ -947,13 +980,14 @@
         <x:item x="12"/>
         <x:item x="13"/>
         <x:item x="14"/>
+        <x:item x="15"/>
       </x:items>
     </x:pivotField>
   </x:pivotFields>
   <x:rowFields count="1">
     <x:field x="4"/>
   </x:rowFields>
-  <x:rowItems count="4">
+  <x:rowItems count="5">
     <x:i>
       <x:x v="0"/>
     </x:i>
@@ -962,6 +996,9 @@
     </x:i>
     <x:i>
       <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
     </x:i>
     <x:i t="grand">
       <x:x/>
@@ -990,7 +1027,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtSort" cacheId="8" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" rowHeaderCaption="Pastry name">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtSort" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1" rowHeaderCaption="Pastry name">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" sortType="ascending" defaultSubtotal="0">
@@ -1006,10 +1043,11 @@
     <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Quality" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Month" axis="axisRow" showAll="0" sortType="descending" defaultSubtotal="0">
-      <x:items count="3">
+      <x:items count="4">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
+        <x:item x="3"/>
       </x:items>
     </x:pivotField>
     <x:pivotField name="BakeDate" defaultSubtotal="0"/>
@@ -1018,7 +1056,7 @@
     <x:field x="0"/>
     <x:field x="4"/>
   </x:rowFields>
-  <x:rowItems count="10">
+  <x:rowItems count="11">
     <x:i>
       <x:x v="0"/>
     </x:i>
@@ -1045,6 +1083,9 @@
     </x:i>
     <x:i>
       <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
     </x:i>
     <x:i t="grand">
       <x:x/>
@@ -1728,7 +1769,7 @@
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="1">
-    <x:tablePart r:id="rId15"/>
+    <x:tablePart r:id="rId17"/>
   </x:tableParts>
 </x:worksheet>
 </file>
@@ -1951,46 +1992,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="1" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems containsBlank="1" count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-        <x:m/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition10.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="1" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5">
+      <x:sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="6">
         <x:n v="101"/>
         <x:n v="102"/>
         <x:n v="103"/>
@@ -2000,297 +2002,22 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems containsBlank="1" count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-        <x:m/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14">
+        <x:n v="150"/>
+        <x:n v="250"/>
+        <x:n v="134"/>
+        <x:n v="225"/>
+        <x:n v="210"/>
+        <x:n v="184"/>
+        <x:n v="124"/>
+        <x:n v="394"/>
+        <x:n v="190"/>
+        <x:n v="221"/>
+        <x:n v="135"/>
+        <x:n v="122"/>
+        <x:n v="243"/>
+        <x:n v="255"/>
       </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15">
-        <x:d v="2016-04-21T00:00:00"/>
-        <x:d v="2016-05-03T00:00:00"/>
-        <x:d v="2016-06-24T00:00:00"/>
-        <x:d v="2017-04-23T00:00:00"/>
-        <x:d v="2016-05-24T00:00:00"/>
-        <x:d v="2016-06-02T00:00:00"/>
-        <x:d v="2016-04-27T00:00:00"/>
-        <x:d v="2016-05-20T00:00:00"/>
-        <x:d v="2017-06-05T00:00:00"/>
-        <x:d v="2017-04-24T00:00:00"/>
-        <x:d v="2017-05-08T00:00:00"/>
-        <x:d v="2016-06-21T00:00:00"/>
-        <x:d v="2017-04-22T00:00:00"/>
-        <x:d v="2017-05-03T00:00:00"/>
-        <x:d v="2017-06-14T00:00:00"/>
-        <x:m/>
-      </x:sharedItems>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="1" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems containsBlank="1" count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-        <x:m/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="1" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems containsBlank="1" count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-        <x:m/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="1" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems containsBlank="1" count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-        <x:m/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="1" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems containsBlank="1" count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-        <x:m/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="1" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems containsBlank="1" count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-        <x:m/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition7.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="1" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems containsBlank="1" count="3">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-        <x:m/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition8.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource name="PastrySalesData"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="1" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
     </x:cacheField>
     <x:cacheField name="Quality">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16">
@@ -2313,7 +2040,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems containsBlank="1" count="3">
+      <x:sharedItems containsBlank="1" count="4">
         <x:s v="Apr"/>
         <x:s v="May"/>
         <x:s v="Jun"/>
@@ -2321,7 +2048,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15">
+      <x:sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="16">
         <x:d v="2016-04-21T00:00:00"/>
         <x:d v="2016-05-03T00:00:00"/>
         <x:d v="2016-06-24T00:00:00"/>
@@ -2344,10 +2071,10 @@
 </x:pivotCacheDefinition>
 </file>
 
-<file path=pivotCache/pivotCacheDefinition9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
+    <x:worksheetSource name="PastrySalesData"/>
   </x:cacheSource>
   <x:cacheFields>
     <x:cacheField name="Name">
@@ -2360,16 +2087,55 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Code">
-      <x:sharedItems containsSemiMixedTypes="1" containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+      <x:sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="6">
+        <x:n v="101"/>
+        <x:n v="102"/>
+        <x:n v="103"/>
+        <x:n v="104"/>
+        <x:n v="105"/>
+        <x:m/>
+      </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14">
+        <x:n v="150"/>
+        <x:n v="250"/>
+        <x:n v="134"/>
+        <x:n v="225"/>
+        <x:n v="210"/>
+        <x:n v="184"/>
+        <x:n v="124"/>
+        <x:n v="394"/>
+        <x:n v="190"/>
+        <x:n v="221"/>
+        <x:n v="135"/>
+        <x:n v="122"/>
+        <x:n v="243"/>
+        <x:n v="255"/>
+      </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16">
+        <x:n v="60.2"/>
+        <x:n v="50.42"/>
+        <x:n v="22.12"/>
+        <x:n v="89.99"/>
+        <x:n v="70"/>
+        <x:n v="75.33"/>
+        <x:n v="10.24"/>
+        <x:n v="33.33"/>
+        <x:n v="25"/>
+        <x:n v="-20.24"/>
+        <x:n v="60"/>
+        <x:n v="24.76"/>
+        <x:n v="0"/>
+        <x:n v="5.19"/>
+        <x:n v="44.2"/>
+        <x:n v="18.4"/>
+      </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems containsBlank="1" count="3">
+      <x:sharedItems containsBlank="1" count="4">
         <x:s v="Apr"/>
         <x:s v="May"/>
         <x:s v="Jun"/>
@@ -2377,7 +2143,24 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="16">
+        <x:d v="2016-04-21T00:00:00"/>
+        <x:d v="2016-05-03T00:00:00"/>
+        <x:d v="2016-06-24T00:00:00"/>
+        <x:d v="2017-04-23T00:00:00"/>
+        <x:d v="2016-05-24T00:00:00"/>
+        <x:d v="2016-06-02T00:00:00"/>
+        <x:d v="2016-04-27T00:00:00"/>
+        <x:d v="2016-05-20T00:00:00"/>
+        <x:d v="2017-06-05T00:00:00"/>
+        <x:d v="2017-04-24T00:00:00"/>
+        <x:d v="2017-05-08T00:00:00"/>
+        <x:d v="2016-06-21T00:00:00"/>
+        <x:d v="2017-04-22T00:00:00"/>
+        <x:d v="2017-05-03T00:00:00"/>
+        <x:d v="2017-06-14T00:00:00"/>
+        <x:m/>
+      </x:sharedItems>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -2387,38 +2170,6 @@
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
-<file path=pivotCache/pivotCacheRecords10.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=pivotCache/pivotCacheRecords4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=pivotCache/pivotCacheRecords5.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=pivotCache/pivotCacheRecords6.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=pivotCache/pivotCacheRecords7.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=pivotCache/pivotCacheRecords8.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=pivotCache/pivotCacheRecords9.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
</xml_diff>

<commit_message>
Save pivot cache records to the output file.
This will ensure, that what was loaded will be saved to the output file. Originally, the cache records were lost and thus any change to the pivot table was impossible for workbooks with changed source (deleted workbook, removed column...). Thanks to round trip load/save, that is no longer the case.

The records for new pivot tables need work, they duplicate values instead of refering to the shared items in pivot cache definition, but Excel can read the records anyway, so it is a significant is progress.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -2155,9 +2155,267 @@
 </file>
 
 <file path=pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="xr">
+  <r>
+    <s v="Croissant"/>
+    <n v="101"/>
+    <n v="150"/>
+    <n v="60.2"/>
+    <s v="Apr"/>
+    <d v="2016-04-21T00:00:00"/>
+  </r>
+  <r>
+    <s v="Croissant"/>
+    <n v="101"/>
+    <n v="250"/>
+    <n v="50.42"/>
+    <s v="May"/>
+    <d v="2016-05-03T00:00:00"/>
+  </r>
+  <r>
+    <s v="Croissant"/>
+    <n v="101"/>
+    <n v="134"/>
+    <n v="22.12"/>
+    <s v="Jun"/>
+    <d v="2016-06-24T00:00:00"/>
+  </r>
+  <r>
+    <s v="Doughnut"/>
+    <n v="102"/>
+    <n v="250"/>
+    <n v="89.99"/>
+    <s v="Apr"/>
+    <d v="2017-04-23T00:00:00"/>
+  </r>
+  <r>
+    <s v="Doughnut"/>
+    <n v="102"/>
+    <n v="225"/>
+    <n v="70"/>
+    <s v="May"/>
+    <d v="2016-05-24T00:00:00"/>
+  </r>
+  <r>
+    <s v="Doughnut"/>
+    <n v="102"/>
+    <n v="210"/>
+    <n v="75.33"/>
+    <s v="Jun"/>
+    <d v="2016-06-02T00:00:00"/>
+  </r>
+  <r>
+    <s v="Bearclaw"/>
+    <n v="103"/>
+    <n v="134"/>
+    <n v="10.24"/>
+    <s v="Apr"/>
+    <d v="2016-04-27T00:00:00"/>
+  </r>
+  <r>
+    <s v="Bearclaw"/>
+    <n v="103"/>
+    <n v="184"/>
+    <n v="33.33"/>
+    <s v="May"/>
+    <d v="2016-05-20T00:00:00"/>
+  </r>
+  <r>
+    <s v="Bearclaw"/>
+    <n v="103"/>
+    <n v="124"/>
+    <n v="25"/>
+    <s v="Jun"/>
+    <d v="2017-06-05T00:00:00"/>
+  </r>
+  <r>
+    <s v="Danish"/>
+    <n v="104"/>
+    <n v="394"/>
+    <n v="-20.24"/>
+    <s v="Apr"/>
+    <d v="2017-04-24T00:00:00"/>
+  </r>
+  <r>
+    <s v="Danish"/>
+    <n v="104"/>
+    <n v="190"/>
+    <n v="60"/>
+    <s v="May"/>
+    <d v="2017-05-08T00:00:00"/>
+  </r>
+  <r>
+    <s v="Danish"/>
+    <n v="104"/>
+    <n v="221"/>
+    <n v="24.76"/>
+    <s v="Jun"/>
+    <d v="2016-06-21T00:00:00"/>
+  </r>
+  <r>
+    <s v="Scone"/>
+    <n v="105"/>
+    <n v="135"/>
+    <n v="0"/>
+    <s v="Apr"/>
+    <d v="2017-04-22T00:00:00"/>
+  </r>
+  <r>
+    <s v="SconE"/>
+    <n v="105"/>
+    <n v="122"/>
+    <n v="5.19"/>
+    <s v="May"/>
+    <d v="2017-05-03T00:00:00"/>
+  </r>
+  <r>
+    <s v="SCONE"/>
+    <n v="105"/>
+    <n v="243"/>
+    <n v="44.2"/>
+    <s v="Jun"/>
+    <d v="2017-06-14T00:00:00"/>
+  </r>
+  <r>
+    <s v="Scone"/>
+    <m/>
+    <n v="255"/>
+    <n v="18.4"/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
 </file>
 
 <file path=pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="xr">
+  <r>
+    <s v="Croissant"/>
+    <n v="101"/>
+    <n v="150"/>
+    <n v="60.2"/>
+    <s v="Apr"/>
+    <d v="2016-04-21T00:00:00"/>
+  </r>
+  <r>
+    <s v="Croissant"/>
+    <n v="101"/>
+    <n v="250"/>
+    <n v="50.42"/>
+    <s v="May"/>
+    <d v="2016-05-03T00:00:00"/>
+  </r>
+  <r>
+    <s v="Croissant"/>
+    <n v="101"/>
+    <n v="134"/>
+    <n v="22.12"/>
+    <s v="Jun"/>
+    <d v="2016-06-24T00:00:00"/>
+  </r>
+  <r>
+    <s v="Doughnut"/>
+    <n v="102"/>
+    <n v="250"/>
+    <n v="89.99"/>
+    <s v="Apr"/>
+    <d v="2017-04-23T00:00:00"/>
+  </r>
+  <r>
+    <s v="Doughnut"/>
+    <n v="102"/>
+    <n v="225"/>
+    <n v="70"/>
+    <s v="May"/>
+    <d v="2016-05-24T00:00:00"/>
+  </r>
+  <r>
+    <s v="Doughnut"/>
+    <n v="102"/>
+    <n v="210"/>
+    <n v="75.33"/>
+    <s v="Jun"/>
+    <d v="2016-06-02T00:00:00"/>
+  </r>
+  <r>
+    <s v="Bearclaw"/>
+    <n v="103"/>
+    <n v="134"/>
+    <n v="10.24"/>
+    <s v="Apr"/>
+    <d v="2016-04-27T00:00:00"/>
+  </r>
+  <r>
+    <s v="Bearclaw"/>
+    <n v="103"/>
+    <n v="184"/>
+    <n v="33.33"/>
+    <s v="May"/>
+    <d v="2016-05-20T00:00:00"/>
+  </r>
+  <r>
+    <s v="Bearclaw"/>
+    <n v="103"/>
+    <n v="124"/>
+    <n v="25"/>
+    <s v="Jun"/>
+    <d v="2017-06-05T00:00:00"/>
+  </r>
+  <r>
+    <s v="Danish"/>
+    <n v="104"/>
+    <n v="394"/>
+    <n v="-20.24"/>
+    <s v="Apr"/>
+    <d v="2017-04-24T00:00:00"/>
+  </r>
+  <r>
+    <s v="Danish"/>
+    <n v="104"/>
+    <n v="190"/>
+    <n v="60"/>
+    <s v="May"/>
+    <d v="2017-05-08T00:00:00"/>
+  </r>
+  <r>
+    <s v="Danish"/>
+    <n v="104"/>
+    <n v="221"/>
+    <n v="24.76"/>
+    <s v="Jun"/>
+    <d v="2016-06-21T00:00:00"/>
+  </r>
+  <r>
+    <s v="Scone"/>
+    <n v="105"/>
+    <n v="135"/>
+    <n v="0"/>
+    <s v="Apr"/>
+    <d v="2017-04-22T00:00:00"/>
+  </r>
+  <r>
+    <s v="SconE"/>
+    <n v="105"/>
+    <n v="122"/>
+    <n v="5.19"/>
+    <s v="May"/>
+    <d v="2017-05-03T00:00:00"/>
+  </r>
+  <r>
+    <s v="SCONE"/>
+    <n v="105"/>
+    <n v="243"/>
+    <n v="44.2"/>
+    <s v="Jun"/>
+    <d v="2017-06-14T00:00:00"/>
+  </r>
+  <r>
+    <s v="Scone"/>
+    <m/>
+    <n v="255"/>
+    <n v="18.4"/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
 </file>
</xml_diff>

<commit_message>
Detach XLPivotSourceReference from actual data.
The source reference might be available, it could be deleted. This allows user to load a workbook even if pivot table uses record data without available source data.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/PivotTables/PivotTables.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/PivotTables/PivotTables.xlsx
@@ -22,7 +22,6 @@
   <x:calcPr calcId="125725"/>
   <x:pivotCaches>
     <x:pivotCache cacheId="0" r:id="rId15"/>
-    <x:pivotCache cacheId="1" r:id="rId16"/>
   </x:pivotCaches>
 </x:workbook>
 </file>
@@ -228,7 +227,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtInteger" cacheId="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtInteger" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -921,7 +920,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFilter" cacheId="1" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvtFilter" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
   <x:location ref="A5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <x:pivotFields count="6">
     <x:pivotField name="Name" axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
@@ -1769,7 +1768,7 @@
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="1">
-    <x:tablePart r:id="rId17"/>
+    <x:tablePart r:id="rId16"/>
   </x:tableParts>
 </x:worksheet>
 </file>
@@ -1965,101 +1964,6 @@
 </file>
 
 <file path=pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
-  <x:cacheSource type="worksheet">
-    <x:worksheetSource ref="A1:F17" sheet="PastrySalesData"/>
-  </x:cacheSource>
-  <x:cacheFields>
-    <x:cacheField name="Name">
-      <x:sharedItems count="5">
-        <x:s v="Croissant"/>
-        <x:s v="Doughnut"/>
-        <x:s v="Bearclaw"/>
-        <x:s v="Danish"/>
-        <x:s v="Scone"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="Code">
-      <x:sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="6">
-        <x:n v="101"/>
-        <x:n v="102"/>
-        <x:n v="103"/>
-        <x:n v="104"/>
-        <x:n v="105"/>
-        <x:m/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="NumberOfOrders">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14">
-        <x:n v="150"/>
-        <x:n v="250"/>
-        <x:n v="134"/>
-        <x:n v="225"/>
-        <x:n v="210"/>
-        <x:n v="184"/>
-        <x:n v="124"/>
-        <x:n v="394"/>
-        <x:n v="190"/>
-        <x:n v="221"/>
-        <x:n v="135"/>
-        <x:n v="122"/>
-        <x:n v="243"/>
-        <x:n v="255"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="Quality">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16">
-        <x:n v="60.2"/>
-        <x:n v="50.42"/>
-        <x:n v="22.12"/>
-        <x:n v="89.99"/>
-        <x:n v="70"/>
-        <x:n v="75.33"/>
-        <x:n v="10.24"/>
-        <x:n v="33.33"/>
-        <x:n v="25"/>
-        <x:n v="-20.24"/>
-        <x:n v="60"/>
-        <x:n v="24.76"/>
-        <x:n v="0"/>
-        <x:n v="5.19"/>
-        <x:n v="44.2"/>
-        <x:n v="18.4"/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="Month">
-      <x:sharedItems containsBlank="1" count="4">
-        <x:s v="Apr"/>
-        <x:s v="May"/>
-        <x:s v="Jun"/>
-        <x:m/>
-      </x:sharedItems>
-    </x:cacheField>
-    <x:cacheField name="BakeDate">
-      <x:sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="16">
-        <x:d v="2016-04-21T00:00:00"/>
-        <x:d v="2016-05-03T00:00:00"/>
-        <x:d v="2016-06-24T00:00:00"/>
-        <x:d v="2017-04-23T00:00:00"/>
-        <x:d v="2016-05-24T00:00:00"/>
-        <x:d v="2016-06-02T00:00:00"/>
-        <x:d v="2016-04-27T00:00:00"/>
-        <x:d v="2016-05-20T00:00:00"/>
-        <x:d v="2017-06-05T00:00:00"/>
-        <x:d v="2017-04-24T00:00:00"/>
-        <x:d v="2017-05-08T00:00:00"/>
-        <x:d v="2016-06-21T00:00:00"/>
-        <x:d v="2017-04-22T00:00:00"/>
-        <x:d v="2017-05-03T00:00:00"/>
-        <x:d v="2017-06-14T00:00:00"/>
-        <x:m/>
-      </x:sharedItems>
-    </x:cacheField>
-  </x:cacheFields>
-</x:pivotCacheDefinition>
-</file>
-
-<file path=pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3">
   <x:cacheSource type="worksheet">
     <x:worksheetSource name="PastrySalesData"/>
@@ -2285,137 +2189,4 @@
     <m/>
   </r>
 </pivotCacheRecords>
-</file>
-
-<file path=pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="xr">
-  <r>
-    <s v="Croissant"/>
-    <n v="101"/>
-    <n v="150"/>
-    <n v="60.2"/>
-    <s v="Apr"/>
-    <d v="2016-04-21T00:00:00"/>
-  </r>
-  <r>
-    <s v="Croissant"/>
-    <n v="101"/>
-    <n v="250"/>
-    <n v="50.42"/>
-    <s v="May"/>
-    <d v="2016-05-03T00:00:00"/>
-  </r>
-  <r>
-    <s v="Croissant"/>
-    <n v="101"/>
-    <n v="134"/>
-    <n v="22.12"/>
-    <s v="Jun"/>
-    <d v="2016-06-24T00:00:00"/>
-  </r>
-  <r>
-    <s v="Doughnut"/>
-    <n v="102"/>
-    <n v="250"/>
-    <n v="89.99"/>
-    <s v="Apr"/>
-    <d v="2017-04-23T00:00:00"/>
-  </r>
-  <r>
-    <s v="Doughnut"/>
-    <n v="102"/>
-    <n v="225"/>
-    <n v="70"/>
-    <s v="May"/>
-    <d v="2016-05-24T00:00:00"/>
-  </r>
-  <r>
-    <s v="Doughnut"/>
-    <n v="102"/>
-    <n v="210"/>
-    <n v="75.33"/>
-    <s v="Jun"/>
-    <d v="2016-06-02T00:00:00"/>
-  </r>
-  <r>
-    <s v="Bearclaw"/>
-    <n v="103"/>
-    <n v="134"/>
-    <n v="10.24"/>
-    <s v="Apr"/>
-    <d v="2016-04-27T00:00:00"/>
-  </r>
-  <r>
-    <s v="Bearclaw"/>
-    <n v="103"/>
-    <n v="184"/>
-    <n v="33.33"/>
-    <s v="May"/>
-    <d v="2016-05-20T00:00:00"/>
-  </r>
-  <r>
-    <s v="Bearclaw"/>
-    <n v="103"/>
-    <n v="124"/>
-    <n v="25"/>
-    <s v="Jun"/>
-    <d v="2017-06-05T00:00:00"/>
-  </r>
-  <r>
-    <s v="Danish"/>
-    <n v="104"/>
-    <n v="394"/>
-    <n v="-20.24"/>
-    <s v="Apr"/>
-    <d v="2017-04-24T00:00:00"/>
-  </r>
-  <r>
-    <s v="Danish"/>
-    <n v="104"/>
-    <n v="190"/>
-    <n v="60"/>
-    <s v="May"/>
-    <d v="2017-05-08T00:00:00"/>
-  </r>
-  <r>
-    <s v="Danish"/>
-    <n v="104"/>
-    <n v="221"/>
-    <n v="24.76"/>
-    <s v="Jun"/>
-    <d v="2016-06-21T00:00:00"/>
-  </r>
-  <r>
-    <s v="Scone"/>
-    <n v="105"/>
-    <n v="135"/>
-    <n v="0"/>
-    <s v="Apr"/>
-    <d v="2017-04-22T00:00:00"/>
-  </r>
-  <r>
-    <s v="SconE"/>
-    <n v="105"/>
-    <n v="122"/>
-    <n v="5.19"/>
-    <s v="May"/>
-    <d v="2017-05-03T00:00:00"/>
-  </r>
-  <r>
-    <s v="SCONE"/>
-    <n v="105"/>
-    <n v="243"/>
-    <n v="44.2"/>
-    <s v="Jun"/>
-    <d v="2017-06-14T00:00:00"/>
-  </r>
-  <r>
-    <s v="Scone"/>
-    <m/>
-    <n v="255"/>
-    <n v="18.4"/>
-    <m/>
-    <m/>
-  </r>
-</pivotCacheRecords>
 </file>
</xml_diff>